<commit_message>
performance stats so far
</commit_message>
<xml_diff>
--- a/apps/libPXGL/examples/performance_graph_sssp.xlsx
+++ b/apps/libPXGL/examples/performance_graph_sssp.xlsx
@@ -13,6 +13,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
+    <t>Nodes=4 Cores=2</t>
+  </si>
+  <si>
     <t>Scale</t>
   </si>
   <si>
@@ -26,6 +29,46 @@
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>Nodes=4 Cores=4</t>
+  </si>
+  <si>
+    <t>
+</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>TEPS</t>
+  </si>
+  <si>
+    <t>Nodes=4 Cores=8</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>TEPS</t>
+  </si>
+  <si>
+    <t>Nodes=3 Cores=2</t>
+  </si>
+  <si>
+    <t>Scale</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>TEPS</t>
   </si>
 </sst>
 </file>
@@ -157,11 +200,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="759340177"/>
-        <c:axId val="1387720144"/>
+        <c:axId val="707480604"/>
+        <c:axId val="1073299479"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="759340177"/>
+        <c:axId val="707480604"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -209,10 +252,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1387720144"/>
+        <c:crossAx val="1073299479"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1387720144"/>
+        <c:axId val="1073299479"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -260,7 +303,196 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="759340177"/>
+        <c:crossAx val="707480604"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="1" sz="1600">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t>Timing (Nodes=4 Cores=4)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$45</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4684EE"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="4684EE"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$46:$C$52</c:f>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$46:$D$52</c:f>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="545353189"/>
+        <c:axId val="1897461419"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="545353189"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>scale(2^x)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt sourceLinked="1" formatCode="General"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1897461419"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1897461419"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt sourceLinked="1" formatCode="General"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="545353189"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -274,7 +506,7 @@
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
   <xdr:absoluteAnchor>
-    <xdr:pos y="3933825" x="4305300"/>
+    <xdr:pos y="3933825" x="4467225"/>
     <xdr:ext cy="3533775" cx="5715000"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -293,6 +525,26 @@
     </xdr:graphicFrame>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:absoluteAnchor>
+  <xdr:absoluteAnchor>
+    <xdr:pos y="8553450" x="6010275"/>
+    <xdr:ext cy="3533775" cx="5715000"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off y="0" x="0"/>
+        <a:ext cy="0" cx="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -302,16 +554,24 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="3" customWidth="1" max="3" width="16.86"/>
+  </cols>
   <sheetData>
+    <row r="5">
+      <c t="s" s="1" r="C5">
+        <v>0</v>
+      </c>
+    </row>
     <row r="7">
       <c t="s" s="1" r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c t="s" s="1" r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c t="s" s="1" r="E7">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
@@ -393,10 +653,10 @@
     </row>
     <row r="21">
       <c t="s" s="1" r="C21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c t="s" s="1" r="D21">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
@@ -453,6 +713,271 @@
       </c>
       <c s="1" r="D28">
         <v>3.568799</v>
+      </c>
+    </row>
+    <row r="43">
+      <c t="s" s="1" r="C43">
+        <v>6</v>
+      </c>
+      <c t="s" s="1" r="D43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45">
+      <c t="s" s="1" r="C45">
+        <v>8</v>
+      </c>
+      <c t="s" s="1" r="D45">
+        <v>9</v>
+      </c>
+      <c t="s" s="1" r="E45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46">
+      <c s="1" r="C46">
+        <v>10.0</v>
+      </c>
+      <c s="1" r="D46">
+        <v>0.1974725</v>
+      </c>
+      <c s="2" r="E46">
+        <v>12716.2141114089</v>
+      </c>
+    </row>
+    <row r="47">
+      <c s="1" r="C47">
+        <v>11.0</v>
+      </c>
+      <c s="1" r="D47">
+        <v>0.3156498</v>
+      </c>
+      <c s="2" r="E47">
+        <v>19480.7612923745</v>
+      </c>
+    </row>
+    <row r="48">
+      <c s="1" r="C48">
+        <v>12.0</v>
+      </c>
+      <c s="1" r="D48">
+        <v>0.4122598</v>
+      </c>
+      <c s="2" r="E48">
+        <v>29187.5731018547</v>
+      </c>
+    </row>
+    <row r="49">
+      <c s="1" r="C49">
+        <v>13.0</v>
+      </c>
+      <c s="1" r="D49">
+        <v>0.7239546</v>
+      </c>
+      <c s="2" r="E49">
+        <v>37054.1807086566</v>
+      </c>
+    </row>
+    <row r="50">
+      <c s="1" r="C50">
+        <v>14.0</v>
+      </c>
+      <c s="1" r="D50">
+        <v>1.3600523</v>
+      </c>
+      <c s="2" r="E50">
+        <v>41395.1712257824</v>
+      </c>
+    </row>
+    <row r="51">
+      <c s="1" r="C51">
+        <v>15.0</v>
+      </c>
+      <c s="1" r="D51">
+        <v>2.8392271</v>
+      </c>
+      <c s="2" r="E51">
+        <v>41411.4027051367</v>
+      </c>
+    </row>
+    <row r="52">
+      <c s="1" r="C52">
+        <v>16.0</v>
+      </c>
+      <c s="1" r="D52">
+        <v>5.9881208</v>
+      </c>
+      <c s="2" r="E52">
+        <v>37907.4982712227</v>
+      </c>
+    </row>
+    <row r="57">
+      <c t="s" s="1" r="C57">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59">
+      <c t="s" s="1" r="C59">
+        <v>12</v>
+      </c>
+      <c t="s" s="1" r="D59">
+        <v>13</v>
+      </c>
+      <c t="s" s="1" r="E59">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60">
+      <c s="1" r="C60">
+        <v>10.0</v>
+      </c>
+      <c s="1" r="D60">
+        <v>0.5359992</v>
+      </c>
+      <c s="2" r="E60">
+        <v>5422.24647210758</v>
+      </c>
+    </row>
+    <row r="61">
+      <c s="1" r="C61">
+        <v>11.0</v>
+      </c>
+      <c s="1" r="D61">
+        <v>0.7315231</v>
+      </c>
+      <c s="2" r="E61">
+        <v>8989.4617562339</v>
+      </c>
+    </row>
+    <row r="62">
+      <c s="1" r="C62">
+        <v>12.0</v>
+      </c>
+      <c s="1" r="D62">
+        <v>0.9159996</v>
+      </c>
+      <c s="2" r="E62">
+        <v>13759.0071727232</v>
+      </c>
+    </row>
+    <row r="63">
+      <c s="1" r="C63">
+        <v>13.0</v>
+      </c>
+      <c s="1" r="D63">
+        <v>1.4399727</v>
+      </c>
+      <c s="2" r="E63">
+        <v>18807.7478029248</v>
+      </c>
+    </row>
+    <row r="64">
+      <c s="1" r="C64">
+        <v>14.0</v>
+      </c>
+      <c s="1" r="D64">
+        <v>2.7086218</v>
+      </c>
+      <c s="2" r="E64">
+        <v>20525.2573975928</v>
+      </c>
+    </row>
+    <row r="65">
+      <c s="1" r="C65">
+        <v>15.0</v>
+      </c>
+      <c s="1" r="D65">
+        <v>5.7760004</v>
+      </c>
+      <c s="2" r="E65">
+        <v>20011.0149927293</v>
+      </c>
+    </row>
+    <row r="66">
+      <c s="1" r="C66">
+        <v>16.0</v>
+      </c>
+      <c s="1" r="D66">
+        <v>12.1160785</v>
+      </c>
+      <c s="2" r="E66">
+        <v>18566.9494157518</v>
+      </c>
+    </row>
+    <row r="71">
+      <c t="s" s="1" r="C71">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73">
+      <c t="s" s="1" r="C73">
+        <v>16</v>
+      </c>
+      <c t="s" s="1" r="D73">
+        <v>17</v>
+      </c>
+      <c t="s" s="1" r="E73">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74">
+      <c s="1" r="C74">
+        <v>10.0</v>
+      </c>
+      <c s="1" r="D74">
+        <v>0.0344298</v>
+      </c>
+      <c s="2" r="E74">
+        <v>101858.335299941</v>
+      </c>
+    </row>
+    <row r="75">
+      <c s="1" r="C75">
+        <v>11.0</v>
+      </c>
+      <c s="1" r="D75">
+        <v>0.0887094</v>
+      </c>
+      <c s="2" r="E75">
+        <v>70881.1862760614</v>
+      </c>
+    </row>
+    <row r="76">
+      <c s="1" r="C76">
+        <v>12.0</v>
+      </c>
+      <c s="1" r="D76">
+        <v>0.3455837</v>
+      </c>
+      <c s="2" r="E76">
+        <v>38056.3543602685</v>
+      </c>
+    </row>
+    <row r="77">
+      <c s="1" r="C77">
+        <v>13.0</v>
+      </c>
+      <c s="1" r="D77">
+        <v>0.8550665</v>
+      </c>
+      <c s="2" r="E77">
+        <v>28896.7091363251</v>
+      </c>
+    </row>
+    <row r="78">
+      <c s="1" r="C78">
+        <v>14.0</v>
+      </c>
+      <c s="1" r="D78"/>
+    </row>
+    <row r="79">
+      <c s="1" r="C79">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c s="1" r="C80">
+        <v>16.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>